<commit_message>
initial commit, Oct 27/2022
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ExcelSheet.xlsx
+++ b/src/test/resources/testData/ExcelSheet.xlsx
@@ -3,35 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7B9B47E9-9845-42C1-A1E5-35E1145C56E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\befis\intellij-workspace\GoogleTNG\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A5494C-1068-4730-9514-4A6C6003B8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1755" windowWidth="38640" windowHeight="15840" tabRatio="618" xr2:uid="{09261A93-1128-465D-B223-0CB4FBF0217C}"/>
+    <workbookView xWindow="0" yWindow="2745" windowWidth="20760" windowHeight="11835" tabRatio="618" xr2:uid="{09261A93-1128-465D-B223-0CB4FBF0217C}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="10" r:id="rId1"/>
     <sheet name="Ref#1" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Values</t>
   </si>
@@ -61,13 +56,19 @@
   </si>
   <si>
     <t>GoogleURL</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Google</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,14 +78,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,16 +100,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0238382-81FA-48F4-A04B-836E7CB4E9D0}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,32 +451,37 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{C0148994-C8F4-44C8-8AE9-BE93745382B4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -495,7 +490,7 @@
           <x14:formula1>
             <xm:f>'Ref#1'!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
+          <xm:sqref>B3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>